<commit_message>
modified incoterm list to make it up-to-date
</commit_message>
<xml_diff>
--- a/catalogue-service-micro/src/test/resources/template/MDF_Raw.xlsx
+++ b/catalogue-service-micro/src/test/resources/template/MDF_Raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\Desktop\Nimble\catalog-service\catalogue-service-micro\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D13D2D9-6D20-41C4-A8DD-BD549EBA28DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D238C34E-6B34-4C79-BFAE-9FB1BFCD9C7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="239">
   <si>
     <t>How to fill in this template?</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>DPU (Delivery at Place Unloaded)</t>
   </si>
 </sst>
 </file>
@@ -847,10 +850,6 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -869,11 +868,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1246,7 +1249,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1256,7 +1259,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1266,17 +1269,17 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1326,7 +1329,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1361,7 +1364,7 @@
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1416,7 +1419,7 @@
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1426,7 +1429,7 @@
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1446,7 +1449,7 @@
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1456,7 +1459,7 @@
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1466,7 +1469,7 @@
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1476,7 +1479,7 @@
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1495,13 +1498,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="5"/>
+    <col min="1" max="1" width="27.109375" style="3"/>
     <col min="2" max="2" width="44.5546875"/>
     <col min="3" max="4" width="25.21875"/>
     <col min="5" max="5" width="21.5546875"/>
@@ -1552,193 +1555,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="19" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="15" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="16"/>
     </row>
     <row r="2" spans="1:52" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="16" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="7" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="7" t="s">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="X2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Y2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AA2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AB2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AC2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AE2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AF2" s="7" t="s">
+      <c r="AF2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AG2" s="7" t="s">
+      <c r="AG2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AH2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AI2" s="7" t="s">
+      <c r="AI2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AJ2" s="7" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AK2" s="7" t="s">
+      <c r="AK2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AL2" s="7" t="s">
+      <c r="AL2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AM2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AN2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AO2" s="7" t="s">
+      <c r="AO2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AP2" s="7" t="s">
+      <c r="AP2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="AQ2" s="7" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="AR2" s="14"/>
-      <c r="AS2" s="7" t="s">
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AT2" s="14"/>
-      <c r="AU2" s="7" t="s">
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="AV2" s="14"/>
-      <c r="AW2" s="7" t="s">
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AX2" s="14"/>
+      <c r="AX2" s="12"/>
       <c r="AY2" t="s">
         <v>90</v>
       </c>
@@ -1747,154 +1750,154 @@
       </c>
     </row>
     <row r="3" spans="1:52" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" s="14" t="s">
+      <c r="M3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="Q3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="S3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="T3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="V3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="X3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF3" s="14" t="s">
+      <c r="Q3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="S3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="AG3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AK3" s="14" t="s">
+      <c r="AG3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AL3" s="14" t="s">
+      <c r="AL3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AM3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AN3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AQ3" s="14" t="s">
+      <c r="AM3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AR3" s="14" t="s">
+      <c r="AR3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AS3" s="14" t="s">
+      <c r="AS3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AT3" s="14" t="s">
+      <c r="AT3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AU3" s="14" t="s">
+      <c r="AU3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AV3" s="14" t="s">
+      <c r="AV3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AW3" s="14" t="s">
+      <c r="AW3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AX3" s="14" t="s">
+      <c r="AX3" s="12" t="s">
         <v>96</v>
       </c>
       <c r="AY3" t="s">
@@ -1905,158 +1908,158 @@
       </c>
     </row>
     <row r="4" spans="1:52" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="14"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="14"/>
-      <c r="AN4" s="14"/>
-      <c r="AO4" s="14"/>
-      <c r="AP4" s="14"/>
-      <c r="AQ4" s="14"/>
-      <c r="AR4" s="14"/>
-      <c r="AS4" s="14"/>
-      <c r="AT4" s="14"/>
-      <c r="AU4" s="14"/>
-      <c r="AV4" s="14"/>
-      <c r="AW4" s="14"/>
-      <c r="AX4" s="14"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="12"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="12"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="12"/>
+      <c r="AV4" s="12"/>
+      <c r="AW4" s="12"/>
+      <c r="AX4" s="12"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="15">
         <v>500</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="11"/>
-      <c r="AL5" s="11"/>
-      <c r="AM5" s="11"/>
-      <c r="AN5" s="11"/>
-      <c r="AO5" s="11"/>
-      <c r="AP5" s="11"/>
-      <c r="AQ5" s="11"/>
-      <c r="AR5" s="11"/>
-      <c r="AS5" s="11"/>
-      <c r="AT5" s="11"/>
-      <c r="AU5" s="11"/>
-      <c r="AV5" s="11"/>
-      <c r="AW5" s="11"/>
-      <c r="AX5" s="11"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
+      <c r="AN5" s="9"/>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="9"/>
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9"/>
+      <c r="AS5" s="9"/>
+      <c r="AT5" s="9"/>
+      <c r="AU5" s="9"/>
+      <c r="AV5" s="9"/>
+      <c r="AW5" s="9"/>
+      <c r="AX5" s="9"/>
       <c r="AY5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>111</v>
       </c>
       <c r="F6" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>112</v>
       </c>
       <c r="H6" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="6" t="s">
         <v>113</v>
       </c>
       <c r="J6" t="s">
@@ -2073,28 +2076,28 @@
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>118</v>
       </c>
       <c r="F7" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>119</v>
       </c>
       <c r="H7" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>120</v>
       </c>
       <c r="J7" t="s">
@@ -2103,7 +2106,7 @@
       <c r="K7">
         <v>100</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="14" t="s">
         <v>237</v>
       </c>
       <c r="AZ7" t="s">
@@ -2143,7 +2146,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="5"/>
+    <col min="1" max="1" width="27.109375" style="3"/>
     <col min="2" max="2" width="44.5546875"/>
     <col min="3" max="3" width="25.21875"/>
     <col min="4" max="4" width="44.21875"/>
@@ -2195,472 +2198,472 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="19" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="15" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="16"/>
     </row>
     <row r="2" spans="1:50" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="16" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="7" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="7" t="s">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="X2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Y2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AA2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AB2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AC2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AE2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AF2" s="7" t="s">
+      <c r="AF2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AG2" s="7" t="s">
+      <c r="AG2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AH2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AI2" s="7" t="s">
+      <c r="AI2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AJ2" s="7" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AK2" s="7" t="s">
+      <c r="AK2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AL2" s="7" t="s">
+      <c r="AL2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AM2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AN2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="AO2" s="7" t="s">
+      <c r="AO2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AP2" s="7" t="s">
+      <c r="AP2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="AQ2" s="7" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="AR2" s="14"/>
-      <c r="AS2" s="7" t="s">
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AT2" s="14"/>
-      <c r="AU2" s="7" t="s">
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="AV2" s="14"/>
-      <c r="AW2" s="7" t="s">
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AX2" s="14"/>
+      <c r="AX2" s="12"/>
     </row>
     <row r="3" spans="1:50" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" s="14" t="s">
+      <c r="M3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="Q3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="S3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="T3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="V3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="X3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF3" s="14" t="s">
+      <c r="Q3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="S3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF3" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="AG3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AK3" s="14" t="s">
+      <c r="AG3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AL3" s="14" t="s">
+      <c r="AL3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AM3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AN3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP3" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AQ3" s="14" t="s">
+      <c r="AM3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AR3" s="14" t="s">
+      <c r="AR3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AS3" s="14" t="s">
+      <c r="AS3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AT3" s="14" t="s">
+      <c r="AT3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AU3" s="14" t="s">
+      <c r="AU3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AV3" s="14" t="s">
+      <c r="AV3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AW3" s="14" t="s">
+      <c r="AW3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AX3" s="14" t="s">
+      <c r="AX3" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:50" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="14"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="14"/>
-      <c r="AN4" s="14"/>
-      <c r="AO4" s="14"/>
-      <c r="AP4" s="14"/>
-      <c r="AQ4" s="14"/>
-      <c r="AR4" s="14"/>
-      <c r="AS4" s="14"/>
-      <c r="AT4" s="14"/>
-      <c r="AU4" s="14"/>
-      <c r="AV4" s="14"/>
-      <c r="AW4" s="14"/>
-      <c r="AX4" s="14"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="12"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="12"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="12"/>
+      <c r="AV4" s="12"/>
+      <c r="AW4" s="12"/>
+      <c r="AX4" s="12"/>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="15">
         <v>500</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="11"/>
-      <c r="AL5" s="11"/>
-      <c r="AM5" s="11"/>
-      <c r="AN5" s="11"/>
-      <c r="AO5" s="11"/>
-      <c r="AP5" s="11"/>
-      <c r="AQ5" s="11"/>
-      <c r="AR5" s="11"/>
-      <c r="AS5" s="11"/>
-      <c r="AT5" s="11"/>
-      <c r="AU5" s="11"/>
-      <c r="AV5" s="11"/>
-      <c r="AW5" s="11"/>
-      <c r="AX5" s="11"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
+      <c r="AN5" s="9"/>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="9"/>
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9"/>
+      <c r="AS5" s="9"/>
+      <c r="AT5" s="9"/>
+      <c r="AU5" s="9"/>
+      <c r="AV5" s="9"/>
+      <c r="AW5" s="9"/>
+      <c r="AX5" s="9"/>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -2672,19 +2675,19 @@
       <c r="D6" t="s">
         <v>110</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>111</v>
       </c>
       <c r="F6" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>112</v>
       </c>
       <c r="H6" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="6" t="s">
         <v>113</v>
       </c>
       <c r="J6" t="s">
@@ -2707,19 +2710,19 @@
       <c r="D7" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>118</v>
       </c>
       <c r="F7" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>119</v>
       </c>
       <c r="H7" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>120</v>
       </c>
       <c r="J7" t="s">
@@ -2728,7 +2731,7 @@
       <c r="K7">
         <v>100</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="14" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2759,13 +2762,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="5"/>
+    <col min="1" max="1" width="27.109375" style="3"/>
     <col min="2" max="2" width="44.5546875"/>
     <col min="3" max="3" width="21.5546875"/>
     <col min="4" max="4" width="14"/>
@@ -2789,283 +2792,283 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="5"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2" t="s">
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="7" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="7" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="U2" s="5"/>
+      <c r="U2" s="3"/>
     </row>
     <row r="3" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="10" t="s">
+      <c r="L5" s="4"/>
+      <c r="M5" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="10" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="R5" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="U5" s="4" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>157</v>
       </c>
       <c r="D6" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>145</v>
       </c>
       <c r="F6" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>147</v>
       </c>
       <c r="H6" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="6" t="s">
         <v>122</v>
       </c>
       <c r="K6" t="s">
         <v>149</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="6" t="s">
         <v>124</v>
       </c>
       <c r="P6" t="s">
         <v>151</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="S6" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="T6" s="8" t="s">
+      <c r="T6" s="6" t="s">
         <v>162</v>
       </c>
       <c r="U6" t="s">
@@ -3073,52 +3076,52 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>145</v>
       </c>
       <c r="D7" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>145</v>
       </c>
       <c r="F7" t="s">
         <v>146</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>163</v>
       </c>
       <c r="H7" t="s">
         <v>146</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="6" t="s">
         <v>125</v>
       </c>
       <c r="K7" t="s">
         <v>149</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="O7" s="8" t="s">
+      <c r="M7" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="O7" s="6" t="s">
         <v>125</v>
       </c>
       <c r="P7" t="s">
         <v>151</v>
       </c>
-      <c r="R7" s="8" t="s">
+      <c r="R7" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="S7" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="T7" s="8" t="s">
+      <c r="T7" s="6" t="s">
         <v>145</v>
       </c>
       <c r="U7" t="s">
@@ -3159,13 +3162,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="5"/>
+    <col min="1" max="1" width="27.109375" style="3"/>
     <col min="2" max="2" width="44.5546875"/>
     <col min="3" max="3" width="21.5546875"/>
     <col min="4" max="4" width="14"/>
@@ -3189,233 +3192,233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="5"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2" t="s">
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="7" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="7" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="U2" s="5"/>
+      <c r="U2" s="3"/>
     </row>
     <row r="3" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S5" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T5" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="U5" s="4" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3507,7 +3510,7 @@
         <v>168</v>
       </c>
       <c r="M7" t="s">
-        <v>164</v>
+        <v>238</v>
       </c>
       <c r="O7" t="s">
         <v>125</v>
@@ -3588,179 +3591,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="10" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="11"/>
       <c r="K2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="19"/>
       <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="F3" s="13"/>
+      <c r="F3" s="11"/>
       <c r="K3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="19"/>
       <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="F4" s="13"/>
+      <c r="F4" s="11"/>
       <c r="K4" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="19"/>
       <c r="B5" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="11"/>
       <c r="K5" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="19"/>
       <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="11"/>
       <c r="K6" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="19"/>
       <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="11"/>
       <c r="K7" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="19"/>
       <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="11"/>
       <c r="K8" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="F9" s="13"/>
+      <c r="F9" s="11"/>
       <c r="K9" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="19"/>
       <c r="B10" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="11"/>
       <c r="K10" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="F11" s="11"/>
       <c r="K11" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="19"/>
       <c r="B12" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="11" t="s">
         <v>193</v>
       </c>
       <c r="K12" t="s">
@@ -3768,14 +3771,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="19"/>
       <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="11" t="s">
         <v>195</v>
       </c>
       <c r="K13" t="s">
@@ -3783,14 +3786,14 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="11" t="s">
         <v>197</v>
       </c>
       <c r="K14" t="s">
@@ -3798,40 +3801,40 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="19"/>
       <c r="B15" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="F15" s="13"/>
+      <c r="F15" s="11"/>
       <c r="K15" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="F16" s="13"/>
+      <c r="F16" s="11"/>
       <c r="K16" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="19"/>
       <c r="B17" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="11" t="s">
         <v>201</v>
       </c>
       <c r="K17" t="s">
@@ -3839,27 +3842,27 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="19"/>
       <c r="B18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="11"/>
       <c r="K18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="11" t="s">
         <v>204</v>
       </c>
       <c r="K19" t="s">
@@ -3867,157 +3870,157 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="19"/>
       <c r="B20" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="F20" s="13"/>
+      <c r="F20" s="11"/>
       <c r="K20" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="19"/>
       <c r="B21" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="F21" s="13"/>
+      <c r="F21" s="11"/>
       <c r="K21" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="19"/>
       <c r="B22" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F22" s="13"/>
+      <c r="F22" s="11"/>
       <c r="K22" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="19"/>
       <c r="B23" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="11"/>
       <c r="K23" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="19"/>
       <c r="B24" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="F24" s="13"/>
+      <c r="F24" s="11"/>
       <c r="K24" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="19"/>
       <c r="B25" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="F25" s="13"/>
+      <c r="F25" s="11"/>
       <c r="K25" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="19"/>
       <c r="B26" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="F26" s="13"/>
+      <c r="F26" s="11"/>
       <c r="K26" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="19"/>
       <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="F27" s="13"/>
+      <c r="F27" s="11"/>
       <c r="K27" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="19"/>
       <c r="B28" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F28" s="13"/>
+      <c r="F28" s="11"/>
       <c r="K28" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="19"/>
       <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="F29" s="13"/>
+      <c r="F29" s="11"/>
       <c r="K29" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="19"/>
       <c r="B30" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="F30" s="13"/>
+      <c r="F30" s="11"/>
       <c r="K30" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="19"/>
       <c r="B31" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="11" t="s">
         <v>216</v>
       </c>
       <c r="K31" t="s">
@@ -4025,40 +4028,40 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="19"/>
       <c r="B32" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="F32" s="13"/>
+      <c r="F32" s="11"/>
       <c r="K32" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="19"/>
       <c r="B33" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="F33" s="13"/>
+      <c r="F33" s="11"/>
       <c r="K33" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+      <c r="A34" s="19"/>
       <c r="B34" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="F34" s="13"/>
+      <c r="F34" s="11"/>
       <c r="K34" t="s">
         <v>186</v>
       </c>

</xml_diff>

<commit_message>
Optimized template upload by using lazy collections
</commit_message>
<xml_diff>
--- a/catalogue-service-micro/src/test/resources/template/MDF_Raw.xlsx
+++ b/catalogue-service-micro/src/test/resources/template/MDF_Raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\Desktop\Nimble\catalog-service\catalogue-service-micro\src\test\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srdc\projects\NIMBLE\project_starts\codes\catalog-service\catalogue-service-micro\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D238C34E-6B34-4C79-BFAE-9FB1BFCD9C7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F8B650-AE82-46D5-9D4B-6B7319294464}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="241">
   <si>
     <t>How to fill in this template?</t>
   </si>
@@ -762,6 +762,12 @@
   </si>
   <si>
     <t>DPU (Delivery at Place Unloaded)</t>
+  </si>
+  <si>
+    <t>Some special terms</t>
+  </si>
+  <si>
+    <t>Warranty info</t>
   </si>
 </sst>
 </file>
@@ -1242,248 +1248,248 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="287.109375"/>
-    <col min="2" max="1025" width="10.77734375"/>
+    <col min="1" max="1" width="287.140625"/>
+    <col min="2" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -1502,59 +1508,59 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="3"/>
-    <col min="2" max="2" width="44.5546875"/>
-    <col min="3" max="4" width="25.21875"/>
-    <col min="5" max="5" width="21.5546875"/>
-    <col min="6" max="6" width="19.44140625"/>
-    <col min="7" max="7" width="21.5546875"/>
-    <col min="8" max="8" width="19.44140625"/>
-    <col min="9" max="9" width="21.5546875"/>
-    <col min="10" max="10" width="19.44140625"/>
-    <col min="11" max="11" width="25.6640625"/>
-    <col min="12" max="12" width="64.6640625"/>
-    <col min="13" max="13" width="51.109375"/>
-    <col min="14" max="14" width="19.44140625"/>
-    <col min="15" max="15" width="30.21875"/>
-    <col min="16" max="16" width="46.44140625"/>
+    <col min="1" max="1" width="27.140625" style="3"/>
+    <col min="2" max="2" width="44.5703125"/>
+    <col min="3" max="4" width="25.28515625"/>
+    <col min="5" max="5" width="21.5703125"/>
+    <col min="6" max="6" width="19.42578125"/>
+    <col min="7" max="7" width="21.5703125"/>
+    <col min="8" max="8" width="19.42578125"/>
+    <col min="9" max="9" width="21.5703125"/>
+    <col min="10" max="10" width="19.42578125"/>
+    <col min="11" max="11" width="25.7109375"/>
+    <col min="12" max="12" width="64.7109375"/>
+    <col min="13" max="13" width="51.140625"/>
+    <col min="14" max="14" width="19.42578125"/>
+    <col min="15" max="15" width="30.28515625"/>
+    <col min="16" max="16" width="46.42578125"/>
     <col min="17" max="17" width="46"/>
-    <col min="18" max="18" width="25.21875"/>
-    <col min="19" max="19" width="36.6640625"/>
-    <col min="20" max="20" width="46.6640625"/>
-    <col min="21" max="21" width="39.77734375"/>
-    <col min="22" max="22" width="54.109375"/>
-    <col min="23" max="23" width="25.21875"/>
-    <col min="24" max="24" width="46.88671875"/>
-    <col min="25" max="25" width="25.21875"/>
-    <col min="26" max="26" width="39.6640625"/>
-    <col min="27" max="27" width="25.21875"/>
+    <col min="18" max="18" width="25.28515625"/>
+    <col min="19" max="19" width="36.7109375"/>
+    <col min="20" max="20" width="46.7109375"/>
+    <col min="21" max="21" width="39.7109375"/>
+    <col min="22" max="22" width="54.140625"/>
+    <col min="23" max="23" width="25.28515625"/>
+    <col min="24" max="24" width="46.85546875"/>
+    <col min="25" max="25" width="25.28515625"/>
+    <col min="26" max="26" width="39.7109375"/>
+    <col min="27" max="27" width="25.28515625"/>
     <col min="28" max="28" width="35"/>
-    <col min="29" max="29" width="27.44140625"/>
-    <col min="30" max="30" width="41.5546875"/>
-    <col min="31" max="31" width="39.109375"/>
-    <col min="32" max="32" width="39.21875"/>
-    <col min="33" max="33" width="32.44140625"/>
-    <col min="34" max="34" width="29.6640625"/>
-    <col min="35" max="35" width="52.33203125"/>
-    <col min="36" max="36" width="37.6640625"/>
-    <col min="37" max="37" width="34.5546875"/>
-    <col min="38" max="38" width="50.6640625"/>
+    <col min="29" max="29" width="27.42578125"/>
+    <col min="30" max="30" width="41.5703125"/>
+    <col min="31" max="31" width="39.140625"/>
+    <col min="32" max="32" width="39.28515625"/>
+    <col min="33" max="33" width="32.42578125"/>
+    <col min="34" max="34" width="29.7109375"/>
+    <col min="35" max="35" width="52.28515625"/>
+    <col min="36" max="36" width="37.7109375"/>
+    <col min="37" max="37" width="34.5703125"/>
+    <col min="38" max="38" width="50.7109375"/>
     <col min="39" max="39" width="34"/>
     <col min="40" max="40" width="37"/>
-    <col min="41" max="41" width="21.5546875"/>
-    <col min="42" max="42" width="19.44140625"/>
-    <col min="43" max="43" width="25.6640625"/>
-    <col min="44" max="44" width="19.44140625"/>
-    <col min="45" max="45" width="21.5546875"/>
-    <col min="46" max="46" width="19.44140625"/>
-    <col min="47" max="47" width="57.6640625"/>
-    <col min="48" max="48" width="19.44140625"/>
-    <col min="49" max="1025" width="10.77734375"/>
+    <col min="41" max="41" width="21.5703125"/>
+    <col min="42" max="42" width="19.42578125"/>
+    <col min="43" max="43" width="25.7109375"/>
+    <col min="44" max="44" width="19.42578125"/>
+    <col min="45" max="45" width="21.5703125"/>
+    <col min="46" max="46" width="19.42578125"/>
+    <col min="47" max="47" width="57.7109375"/>
+    <col min="48" max="48" width="19.42578125"/>
+    <col min="49" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1609,7 +1615,7 @@
       <c r="AW1" s="16"/>
       <c r="AX1" s="16"/>
     </row>
-    <row r="2" spans="1:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -1749,7 +1755,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
@@ -1907,7 +1913,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
@@ -1961,7 +1967,7 @@
       <c r="AW4" s="12"/>
       <c r="AX4" s="12"/>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>100</v>
       </c>
@@ -2037,7 +2043,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>108</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>115</v>
       </c>
@@ -2144,60 +2150,60 @@
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="3"/>
-    <col min="2" max="2" width="44.5546875"/>
-    <col min="3" max="3" width="25.21875"/>
-    <col min="4" max="4" width="44.21875"/>
-    <col min="5" max="5" width="21.5546875"/>
-    <col min="6" max="6" width="19.44140625"/>
-    <col min="7" max="7" width="21.5546875"/>
-    <col min="8" max="8" width="19.44140625"/>
-    <col min="9" max="9" width="21.5546875"/>
-    <col min="10" max="10" width="19.44140625"/>
-    <col min="11" max="11" width="25.6640625"/>
-    <col min="12" max="12" width="64.6640625"/>
-    <col min="13" max="13" width="51.109375"/>
-    <col min="14" max="14" width="19.44140625"/>
-    <col min="15" max="15" width="30.21875"/>
-    <col min="16" max="16" width="46.44140625"/>
+    <col min="1" max="1" width="27.140625" style="3"/>
+    <col min="2" max="2" width="44.5703125"/>
+    <col min="3" max="3" width="25.28515625"/>
+    <col min="4" max="4" width="44.28515625"/>
+    <col min="5" max="5" width="21.5703125"/>
+    <col min="6" max="6" width="19.42578125"/>
+    <col min="7" max="7" width="21.5703125"/>
+    <col min="8" max="8" width="19.42578125"/>
+    <col min="9" max="9" width="21.5703125"/>
+    <col min="10" max="10" width="19.42578125"/>
+    <col min="11" max="11" width="25.7109375"/>
+    <col min="12" max="12" width="64.7109375"/>
+    <col min="13" max="13" width="51.140625"/>
+    <col min="14" max="14" width="19.42578125"/>
+    <col min="15" max="15" width="30.28515625"/>
+    <col min="16" max="16" width="46.42578125"/>
     <col min="17" max="17" width="46"/>
-    <col min="18" max="18" width="25.21875"/>
-    <col min="19" max="19" width="36.6640625"/>
-    <col min="20" max="20" width="46.6640625"/>
-    <col min="21" max="21" width="39.77734375"/>
-    <col min="22" max="22" width="54.109375"/>
-    <col min="23" max="23" width="25.21875"/>
-    <col min="24" max="24" width="46.88671875"/>
-    <col min="25" max="25" width="25.21875"/>
-    <col min="26" max="26" width="39.6640625"/>
-    <col min="27" max="27" width="25.21875"/>
+    <col min="18" max="18" width="25.28515625"/>
+    <col min="19" max="19" width="36.7109375"/>
+    <col min="20" max="20" width="46.7109375"/>
+    <col min="21" max="21" width="39.7109375"/>
+    <col min="22" max="22" width="54.140625"/>
+    <col min="23" max="23" width="25.28515625"/>
+    <col min="24" max="24" width="46.85546875"/>
+    <col min="25" max="25" width="25.28515625"/>
+    <col min="26" max="26" width="39.7109375"/>
+    <col min="27" max="27" width="25.28515625"/>
     <col min="28" max="28" width="35"/>
-    <col min="29" max="29" width="27.44140625"/>
-    <col min="30" max="30" width="41.5546875"/>
-    <col min="31" max="31" width="39.109375"/>
-    <col min="32" max="32" width="39.21875"/>
-    <col min="33" max="33" width="32.44140625"/>
-    <col min="34" max="34" width="29.6640625"/>
-    <col min="35" max="35" width="52.33203125"/>
-    <col min="36" max="36" width="37.6640625"/>
-    <col min="37" max="37" width="34.5546875"/>
-    <col min="38" max="38" width="50.6640625"/>
+    <col min="29" max="29" width="27.42578125"/>
+    <col min="30" max="30" width="41.5703125"/>
+    <col min="31" max="31" width="39.140625"/>
+    <col min="32" max="32" width="39.28515625"/>
+    <col min="33" max="33" width="32.42578125"/>
+    <col min="34" max="34" width="29.7109375"/>
+    <col min="35" max="35" width="52.28515625"/>
+    <col min="36" max="36" width="37.7109375"/>
+    <col min="37" max="37" width="34.5703125"/>
+    <col min="38" max="38" width="50.7109375"/>
     <col min="39" max="39" width="34"/>
     <col min="40" max="40" width="37"/>
-    <col min="41" max="41" width="21.5546875"/>
-    <col min="42" max="42" width="19.44140625"/>
-    <col min="43" max="43" width="25.6640625"/>
-    <col min="44" max="44" width="19.44140625"/>
-    <col min="45" max="45" width="21.5546875"/>
-    <col min="46" max="46" width="19.44140625"/>
-    <col min="47" max="47" width="57.6640625"/>
-    <col min="48" max="48" width="19.44140625"/>
-    <col min="49" max="1025" width="10.77734375"/>
+    <col min="41" max="41" width="21.5703125"/>
+    <col min="42" max="42" width="19.42578125"/>
+    <col min="43" max="43" width="25.7109375"/>
+    <col min="44" max="44" width="19.42578125"/>
+    <col min="45" max="45" width="21.5703125"/>
+    <col min="46" max="46" width="19.42578125"/>
+    <col min="47" max="47" width="57.7109375"/>
+    <col min="48" max="48" width="19.42578125"/>
+    <col min="49" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2252,7 +2258,7 @@
       <c r="AW1" s="16"/>
       <c r="AX1" s="16"/>
     </row>
-    <row r="2" spans="1:50" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -2386,7 +2392,7 @@
       </c>
       <c r="AX2" s="12"/>
     </row>
-    <row r="3" spans="1:50" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
@@ -2538,7 +2544,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
@@ -2592,7 +2598,7 @@
       <c r="AW4" s="12"/>
       <c r="AX4" s="12"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>100</v>
       </c>
@@ -2665,7 +2671,7 @@
       <c r="AW5" s="9"/>
       <c r="AX5" s="9"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>108</v>
       </c>
@@ -2700,7 +2706,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>115</v>
       </c>
@@ -2766,32 +2772,32 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="3"/>
-    <col min="2" max="2" width="44.5546875"/>
-    <col min="3" max="3" width="21.5546875"/>
+    <col min="1" max="1" width="27.140625" style="3"/>
+    <col min="2" max="2" width="44.5703125"/>
+    <col min="3" max="3" width="21.5703125"/>
     <col min="4" max="4" width="14"/>
-    <col min="5" max="5" width="27.5546875"/>
-    <col min="6" max="6" width="19.44140625"/>
-    <col min="7" max="7" width="34.109375"/>
-    <col min="8" max="8" width="19.44140625"/>
-    <col min="9" max="9" width="17.77734375"/>
+    <col min="5" max="5" width="27.5703125"/>
+    <col min="6" max="6" width="19.42578125"/>
+    <col min="7" max="7" width="34.140625"/>
+    <col min="8" max="8" width="19.42578125"/>
+    <col min="9" max="9" width="17.7109375"/>
     <col min="10" max="10" width="34"/>
-    <col min="11" max="11" width="19.44140625"/>
-    <col min="12" max="12" width="30.109375"/>
-    <col min="13" max="13" width="14.5546875"/>
-    <col min="14" max="14" width="19.88671875"/>
-    <col min="15" max="15" width="35.6640625"/>
-    <col min="16" max="16" width="19.44140625"/>
-    <col min="17" max="17" width="37.88671875"/>
-    <col min="18" max="19" width="22.21875"/>
-    <col min="20" max="20" width="24.6640625"/>
-    <col min="21" max="21" width="19.44140625"/>
-    <col min="22" max="1025" width="10.77734375"/>
+    <col min="11" max="11" width="19.42578125"/>
+    <col min="12" max="12" width="30.140625"/>
+    <col min="13" max="13" width="14.5703125"/>
+    <col min="14" max="14" width="19.85546875"/>
+    <col min="15" max="15" width="35.7109375"/>
+    <col min="16" max="16" width="19.42578125"/>
+    <col min="17" max="17" width="37.85546875"/>
+    <col min="18" max="19" width="22.28515625"/>
+    <col min="20" max="20" width="24.7109375"/>
+    <col min="21" max="21" width="19.42578125"/>
+    <col min="22" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="18" t="s">
         <v>126</v>
@@ -2821,7 +2827,7 @@
       <c r="T1" s="18"/>
       <c r="U1" s="18"/>
     </row>
-    <row r="2" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -2874,7 +2880,7 @@
       </c>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
@@ -2939,7 +2945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
@@ -2964,7 +2970,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>100</v>
       </c>
@@ -3022,7 +3028,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>108</v>
       </c>
@@ -3075,7 +3081,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>115</v>
       </c>
@@ -3162,36 +3168,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="3"/>
-    <col min="2" max="2" width="44.5546875"/>
-    <col min="3" max="3" width="21.5546875"/>
+    <col min="1" max="1" width="27.140625" style="3"/>
+    <col min="2" max="2" width="44.5703125"/>
+    <col min="3" max="3" width="21.5703125"/>
     <col min="4" max="4" width="14"/>
-    <col min="5" max="5" width="27.5546875"/>
-    <col min="6" max="6" width="19.44140625"/>
-    <col min="7" max="7" width="34.109375"/>
-    <col min="8" max="8" width="19.44140625"/>
-    <col min="9" max="9" width="17.77734375"/>
+    <col min="5" max="5" width="27.5703125"/>
+    <col min="6" max="6" width="19.42578125"/>
+    <col min="7" max="7" width="34.140625"/>
+    <col min="8" max="8" width="19.42578125"/>
+    <col min="9" max="9" width="17.7109375"/>
     <col min="10" max="10" width="34"/>
-    <col min="11" max="11" width="19.44140625"/>
-    <col min="12" max="12" width="30.109375"/>
-    <col min="13" max="13" width="38.88671875"/>
-    <col min="14" max="14" width="19.88671875"/>
-    <col min="15" max="15" width="35.6640625"/>
-    <col min="16" max="16" width="19.44140625"/>
-    <col min="17" max="17" width="37.88671875"/>
-    <col min="18" max="19" width="22.21875"/>
-    <col min="20" max="20" width="24.6640625"/>
-    <col min="21" max="21" width="19.44140625"/>
-    <col min="22" max="1025" width="10.77734375"/>
+    <col min="11" max="11" width="19.42578125"/>
+    <col min="12" max="12" width="30.140625"/>
+    <col min="13" max="13" width="38.85546875"/>
+    <col min="14" max="14" width="19.85546875"/>
+    <col min="15" max="15" width="35.7109375"/>
+    <col min="16" max="16" width="19.42578125"/>
+    <col min="17" max="17" width="37.85546875"/>
+    <col min="18" max="19" width="22.28515625"/>
+    <col min="20" max="20" width="24.7109375"/>
+    <col min="21" max="21" width="19.42578125"/>
+    <col min="22" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="18" t="s">
         <v>126</v>
@@ -3221,7 +3227,7 @@
       <c r="T1" s="18"/>
       <c r="U1" s="18"/>
     </row>
-    <row r="2" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -3274,7 +3280,7 @@
       </c>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
@@ -3339,7 +3345,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
@@ -3364,7 +3370,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>100</v>
       </c>
@@ -3422,7 +3428,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>108</v>
       </c>
@@ -3453,9 +3459,15 @@
       <c r="K6" t="s">
         <v>168</v>
       </c>
+      <c r="L6" t="s">
+        <v>240</v>
+      </c>
       <c r="M6" t="s">
         <v>159</v>
       </c>
+      <c r="N6" t="s">
+        <v>239</v>
+      </c>
       <c r="O6" t="s">
         <v>124</v>
       </c>
@@ -3478,7 +3490,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>115</v>
       </c>
@@ -3574,23 +3586,23 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.21875"/>
-    <col min="2" max="2" width="56.6640625"/>
+    <col min="1" max="1" width="14.28515625"/>
+    <col min="2" max="2" width="56.7109375"/>
     <col min="3" max="3" width="17"/>
-    <col min="4" max="4" width="63.5546875"/>
-    <col min="5" max="5" width="7.6640625"/>
-    <col min="6" max="6" width="63.5546875"/>
-    <col min="7" max="7" width="24.5546875"/>
-    <col min="8" max="8" width="6.88671875"/>
-    <col min="9" max="9" width="18.33203125"/>
-    <col min="10" max="10" width="20.5546875"/>
-    <col min="11" max="11" width="14.6640625"/>
-    <col min="12" max="1025" width="10.77734375"/>
+    <col min="4" max="4" width="63.5703125"/>
+    <col min="5" max="5" width="7.7109375"/>
+    <col min="6" max="6" width="63.5703125"/>
+    <col min="7" max="7" width="24.5703125"/>
+    <col min="8" max="8" width="6.85546875"/>
+    <col min="9" max="9" width="18.28515625"/>
+    <col min="10" max="10" width="20.5703125"/>
+    <col min="11" max="11" width="14.7109375"/>
+    <col min="12" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
         <v>50</v>
@@ -3623,7 +3635,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>49</v>
       </c>
@@ -3638,7 +3650,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" t="s">
         <v>58</v>
@@ -3651,7 +3663,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" t="s">
         <v>59</v>
@@ -3664,7 +3676,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" t="s">
         <v>60</v>
@@ -3677,7 +3689,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" t="s">
         <v>61</v>
@@ -3690,7 +3702,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" t="s">
         <v>62</v>
@@ -3703,7 +3715,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" t="s">
         <v>63</v>
@@ -3716,7 +3728,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>64</v>
@@ -3729,7 +3741,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" t="s">
         <v>65</v>
@@ -3742,7 +3754,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>66</v>
@@ -3755,7 +3767,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" t="s">
         <v>67</v>
@@ -3770,7 +3782,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" t="s">
         <v>68</v>
@@ -3785,7 +3797,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>69</v>
@@ -3800,7 +3812,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" t="s">
         <v>70</v>
@@ -3813,7 +3825,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>71</v>
@@ -3826,7 +3838,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" t="s">
         <v>72</v>
@@ -3841,7 +3853,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" t="s">
         <v>73</v>
@@ -3854,7 +3866,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>74</v>
@@ -3869,7 +3881,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" t="s">
         <v>75</v>
@@ -3882,7 +3894,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" t="s">
         <v>76</v>
@@ -3895,7 +3907,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" t="s">
         <v>77</v>
@@ -3908,7 +3920,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" t="s">
         <v>78</v>
@@ -3921,7 +3933,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" t="s">
         <v>79</v>
@@ -3934,7 +3946,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" t="s">
         <v>80</v>
@@ -3947,7 +3959,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" t="s">
         <v>81</v>
@@ -3960,7 +3972,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" t="s">
         <v>82</v>
@@ -3973,7 +3985,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" t="s">
         <v>83</v>
@@ -3986,7 +3998,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" t="s">
         <v>84</v>
@@ -3999,7 +4011,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
       <c r="B30" t="s">
         <v>85</v>
@@ -4012,7 +4024,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" t="s">
         <v>86</v>
@@ -4027,7 +4039,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" t="s">
         <v>87</v>
@@ -4040,7 +4052,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
       <c r="B33" t="s">
         <v>88</v>
@@ -4053,7 +4065,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" t="s">
         <v>89</v>
@@ -4081,9 +4093,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.77734375"/>
+    <col min="1" max="1025" width="10.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4097,22 +4109,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.77734375"/>
+    <col min="1" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -4129,12 +4141,12 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.77734375"/>
+    <col min="1" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>223</v>
       </c>
@@ -4154,7 +4166,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -4174,7 +4186,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -4194,7 +4206,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>228</v>
       </c>
@@ -4208,42 +4220,42 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>159</v>
       </c>

</xml_diff>

<commit_message>
remove product status from the template upload
</commit_message>
<xml_diff>
--- a/catalogue-service-micro/src/test/resources/template/MDF_Raw.xlsx
+++ b/catalogue-service-micro/src/test/resources/template/MDF_Raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\Desktop\Nimble\catalog-service\catalogue-service-micro\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817E993F-339A-41B7-812C-6B1D1F83AFE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF78406-22C3-4AA7-B748-9D222C58E490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="241">
   <si>
     <t>How to fill in this template?</t>
   </si>
@@ -768,12 +768,6 @@
   </si>
   <si>
     <t>Warranty info</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>PUBLISHED</t>
   </si>
 </sst>
 </file>
@@ -885,8 +879,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1510,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BA7"/>
+  <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1568,63 +1562,62 @@
     <col min="49" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="18" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-    </row>
-    <row r="2" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="16"/>
+    </row>
+    <row r="2" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -1637,135 +1630,132 @@
       <c r="D2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="16" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="16" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="13" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="M2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="N2" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="16" t="s">
+        <v>60</v>
+      </c>
       <c r="R2" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U2" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="V2" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="W2" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="X2" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Y2" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z2" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AA2" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AB2" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AC2" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AD2" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE2" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AF2" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AG2" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AH2" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AI2" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AJ2" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AK2" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AL2" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AM2" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AN2" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AO2" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AP2" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AQ2" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR2" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="16" t="s">
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="AU2" s="12"/>
-      <c r="AV2" s="16" t="s">
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="16" t="s">
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AY2" s="12"/>
+      <c r="AX2" s="12"/>
+      <c r="AY2" t="s">
+        <v>90</v>
+      </c>
       <c r="AZ2" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
@@ -1779,43 +1769,43 @@
         <v>94</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="P3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="N3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>95</v>
-      </c>
       <c r="Q3" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R3" s="12" t="s">
         <v>94</v>
@@ -1860,10 +1850,10 @@
         <v>94</v>
       </c>
       <c r="AF3" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AH3" s="12" t="s">
         <v>94</v>
@@ -1875,13 +1865,13 @@
         <v>94</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="AL3" s="12" t="s">
         <v>98</v>
       </c>
       <c r="AM3" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="AN3" s="12" t="s">
         <v>94</v>
@@ -1893,40 +1883,37 @@
         <v>94</v>
       </c>
       <c r="AQ3" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AR3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AS3" s="12" t="s">
+      <c r="AT3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AT3" s="12" t="s">
+      <c r="AU3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AU3" s="12" t="s">
+      <c r="AV3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AV3" s="12" t="s">
+      <c r="AW3" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AW3" s="12" t="s">
+      <c r="AX3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AX3" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="AY3" s="12" t="s">
-        <v>96</v>
+      <c r="AY3" t="s">
+        <v>94</v>
       </c>
       <c r="AZ3" t="s">
         <v>94</v>
       </c>
-      <c r="BA3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
@@ -1939,9 +1926,9 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
@@ -1979,9 +1966,8 @@
       <c r="AV4" s="12"/>
       <c r="AW4" s="12"/>
       <c r="AX4" s="12"/>
-      <c r="AY4" s="12"/>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>100</v>
       </c>
@@ -1992,32 +1978,30 @@
         <v>102</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="F5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="15">
+      <c r="K5" s="15">
         <v>500</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="L5" s="15" t="s">
         <v>237</v>
       </c>
+      <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
@@ -2055,12 +2039,11 @@
       <c r="AV5" s="9"/>
       <c r="AW5" s="9"/>
       <c r="AX5" s="9"/>
-      <c r="AY5" s="9"/>
-      <c r="AZ5" t="s">
+      <c r="AY5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>108</v>
       </c>
@@ -2070,38 +2053,35 @@
       <c r="D6" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
         <v>104</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
         <v>104</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6" t="s">
         <v>104</v>
       </c>
-      <c r="L6">
+      <c r="K6">
         <v>200</v>
       </c>
-      <c r="M6" t="s">
+      <c r="L6" t="s">
         <v>237</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="AZ6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>115</v>
       </c>
@@ -2111,52 +2091,45 @@
       <c r="D7" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" t="s">
         <v>104</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7" t="s">
         <v>104</v>
       </c>
-      <c r="L7">
+      <c r="K7">
         <v>100</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="L7" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="BA7" t="s">
+      <c r="AZ7" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="N1:AY1"/>
-  </mergeCells>
   <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid input !" error="Please, select one of the available options" sqref="G5 K5 I5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid input !" error="Please, select one of the available options" sqref="F5 J5 H5" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>Dimension</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid input !" error="Please, select one of the available options" sqref="AL5:AM5" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid input !" error="Please, select one of the available options" sqref="AK5:AL5" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>Boolean</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid input !" error="Please, select one of the available options" sqref="M5" xr:uid="{392C2D04-1CCF-461A-8534-2B10F521D8EA}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid input !" error="Please, select one of the available options" sqref="L5" xr:uid="{392C2D04-1CCF-461A-8534-2B10F521D8EA}">
       <formula1>Weight</formula1>
     </dataValidation>
   </dataValidations>
@@ -2230,56 +2203,56 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="18" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
+      <c r="AV1" s="19"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="19"/>
     </row>
     <row r="2" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">

</xml_diff>

<commit_message>
remove applicable address country from indexing and template publishing
</commit_message>
<xml_diff>
--- a/catalogue-service-micro/src/test/resources/template/MDF_Raw.xlsx
+++ b/catalogue-service-micro/src/test/resources/template/MDF_Raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\Desktop\Nimble\catalog-service\catalogue-service-micro\src\test\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF78406-22C3-4AA7-B748-9D222C58E490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5562A600-D63F-494E-99B6-0C7279C63C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="241">
   <si>
     <t>How to fill in this template?</t>
   </si>
@@ -854,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -879,6 +879,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1506,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -2203,56 +2206,56 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="19" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="19"/>
-      <c r="AU1" s="19"/>
-      <c r="AV1" s="19"/>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="19"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
     </row>
     <row r="2" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2762,10 +2765,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2793,37 +2796,36 @@
     <col min="22" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20" t="s">
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="20" t="s">
         <v>129</v>
       </c>
+      <c r="S1" s="20"/>
       <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-    </row>
-    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
@@ -2863,20 +2865,17 @@
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="R2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="R2" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="S2" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="U2" s="3"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
@@ -2932,16 +2931,13 @@
         <v>93</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="U3" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>99</v>
       </c>
@@ -2964,9 +2960,8 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>100</v>
       </c>
@@ -3009,22 +3004,19 @@
         <v>151</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="T5" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>108</v>
       </c>
@@ -3064,20 +3056,20 @@
       <c r="P6" t="s">
         <v>151</v>
       </c>
+      <c r="Q6" s="6" t="s">
+        <v>160</v>
+      </c>
       <c r="R6" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="T6" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="U6" t="s">
+      <c r="T6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>115</v>
       </c>
@@ -3117,25 +3109,23 @@
       <c r="P7" t="s">
         <v>151</v>
       </c>
+      <c r="Q7" s="6" t="s">
+        <v>160</v>
+      </c>
       <c r="R7" s="6" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="T7" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="U7" t="s">
+      <c r="T7" t="s">
         <v>156</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="S1:U1"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid input !" error="Please, select one of the available options" sqref="D5" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -3195,33 +3185,33 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20" t="s">
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
     </row>
     <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3632,7 +3622,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B2" t="s">
@@ -3647,7 +3637,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
+      <c r="A3" s="24"/>
       <c r="B3" t="s">
         <v>58</v>
       </c>
@@ -3660,7 +3650,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
+      <c r="A4" s="24"/>
       <c r="B4" t="s">
         <v>59</v>
       </c>
@@ -3673,7 +3663,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
+      <c r="A5" s="24"/>
       <c r="B5" t="s">
         <v>60</v>
       </c>
@@ -3686,7 +3676,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
+      <c r="A6" s="24"/>
       <c r="B6" t="s">
         <v>61</v>
       </c>
@@ -3699,7 +3689,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="24"/>
       <c r="B7" t="s">
         <v>62</v>
       </c>
@@ -3712,7 +3702,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="24"/>
       <c r="B8" t="s">
         <v>63</v>
       </c>
@@ -3725,7 +3715,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
+      <c r="A9" s="24"/>
       <c r="B9" t="s">
         <v>64</v>
       </c>
@@ -3738,7 +3728,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
+      <c r="A10" s="24"/>
       <c r="B10" t="s">
         <v>65</v>
       </c>
@@ -3751,7 +3741,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
+      <c r="A11" s="24"/>
       <c r="B11" t="s">
         <v>66</v>
       </c>
@@ -3764,7 +3754,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
+      <c r="A12" s="24"/>
       <c r="B12" t="s">
         <v>67</v>
       </c>
@@ -3779,7 +3769,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
+      <c r="A13" s="24"/>
       <c r="B13" t="s">
         <v>68</v>
       </c>
@@ -3794,7 +3784,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
+      <c r="A14" s="24"/>
       <c r="B14" t="s">
         <v>69</v>
       </c>
@@ -3809,7 +3799,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
+      <c r="A15" s="24"/>
       <c r="B15" t="s">
         <v>70</v>
       </c>
@@ -3822,7 +3812,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
+      <c r="A16" s="24"/>
       <c r="B16" t="s">
         <v>71</v>
       </c>
@@ -3835,7 +3825,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
+      <c r="A17" s="24"/>
       <c r="B17" t="s">
         <v>72</v>
       </c>
@@ -3850,7 +3840,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
+      <c r="A18" s="24"/>
       <c r="B18" t="s">
         <v>73</v>
       </c>
@@ -3863,7 +3853,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
+      <c r="A19" s="24"/>
       <c r="B19" t="s">
         <v>74</v>
       </c>
@@ -3878,7 +3868,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
+      <c r="A20" s="24"/>
       <c r="B20" t="s">
         <v>75</v>
       </c>
@@ -3891,7 +3881,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
+      <c r="A21" s="24"/>
       <c r="B21" t="s">
         <v>76</v>
       </c>
@@ -3904,7 +3894,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
+      <c r="A22" s="24"/>
       <c r="B22" t="s">
         <v>77</v>
       </c>
@@ -3917,7 +3907,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
+      <c r="A23" s="24"/>
       <c r="B23" t="s">
         <v>78</v>
       </c>
@@ -3930,7 +3920,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
+      <c r="A24" s="24"/>
       <c r="B24" t="s">
         <v>79</v>
       </c>
@@ -3943,7 +3933,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
+      <c r="A25" s="24"/>
       <c r="B25" t="s">
         <v>80</v>
       </c>
@@ -3956,7 +3946,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
+      <c r="A26" s="24"/>
       <c r="B26" t="s">
         <v>81</v>
       </c>
@@ -3969,7 +3959,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
+      <c r="A27" s="24"/>
       <c r="B27" t="s">
         <v>82</v>
       </c>
@@ -3982,7 +3972,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
+      <c r="A28" s="24"/>
       <c r="B28" t="s">
         <v>83</v>
       </c>
@@ -3995,7 +3985,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
+      <c r="A29" s="24"/>
       <c r="B29" t="s">
         <v>84</v>
       </c>
@@ -4008,7 +3998,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
+      <c r="A30" s="24"/>
       <c r="B30" t="s">
         <v>85</v>
       </c>
@@ -4021,7 +4011,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
+      <c r="A31" s="24"/>
       <c r="B31" t="s">
         <v>86</v>
       </c>
@@ -4036,7 +4026,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
+      <c r="A32" s="24"/>
       <c r="B32" t="s">
         <v>87</v>
       </c>
@@ -4049,7 +4039,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
+      <c r="A33" s="24"/>
       <c r="B33" t="s">
         <v>88</v>
       </c>
@@ -4062,7 +4052,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
+      <c r="A34" s="24"/>
       <c r="B34" t="s">
         <v>89</v>
       </c>

</xml_diff>